<commit_message>
Added changes to support azure pipeline
</commit_message>
<xml_diff>
--- a/src/test/java/resources/data/TestData.xlsx
+++ b/src/test/java/resources/data/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="171">
   <si>
     <t>#</t>
   </si>
@@ -551,6 +551,18 @@
   </si>
   <si>
     <t>22.94</t>
+  </si>
+  <si>
+    <t>14010</t>
+  </si>
+  <si>
+    <t>21.38</t>
+  </si>
+  <si>
+    <t>15120</t>
+  </si>
+  <si>
+    <t>44.47</t>
   </si>
 </sst>
 </file>
@@ -1745,7 +1757,7 @@
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
@@ -1798,13 +1810,13 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="AB16" s="1" t="s">
         <v>68</v>
@@ -2351,16 +2363,16 @@
         <v>139</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="Z25" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>

</xml_diff>